<commit_message>
Distinguish case where name is not in NCBI
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -203,12 +203,12 @@
     </comment>
     <comment authorId="1" ref="AA11" shapeId="0">
       <text>
-        <t>Not a virus</t>
+        <t>Not found in NCBI Taxonomy`</t>
       </text>
     </comment>
     <comment authorId="1" ref="AA12" shapeId="0">
       <text>
-        <t>Not a virus</t>
+        <t>Not found in NCBI Taxonomy`</t>
       </text>
     </comment>
   </commentList>
@@ -759,7 +759,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill/>
     </fill>
@@ -844,6 +844,12 @@
         <bgColor rgb="00FFD8D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFBBBB"/>
+        <bgColor rgb="00FFBBBB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -911,11 +917,11 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -978,11 +984,14 @@
     <xf applyAlignment="1" borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -1319,7 +1328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1340,571 +1349,571 @@
     <col customWidth="1" max="29" min="28" width="13.5"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="38.25" r="1" spans="1:29">
-      <c r="A1" s="2" t="s">
+    <row spans="1:29" customHeight="1" ht="38.25" r="1">
+      <c t="s" r="A1" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c t="s" r="B1" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c t="s" r="C1" s="2">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="51" r="2" spans="1:29">
-      <c r="A2" s="1" t="s">
+    <row spans="1:29" customHeight="1" ht="51" r="2">
+      <c t="s" r="A2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="63.75" r="3" spans="1:29">
-      <c r="A3" s="4" t="s">
+    <row spans="1:29" customHeight="1" ht="63.75" r="3">
+      <c t="s" r="A3" s="4">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c t="s" r="B3" s="7">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c t="s" r="C3" s="9">
         <v>6</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c t="s" r="D3" s="11">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c t="s" r="E3" s="7">
         <v>8</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c t="s" r="F3" s="7">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c t="s" r="G3" s="6">
         <v>10</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c t="s" r="H3" s="6">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c t="s" r="I3" s="6">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c t="s" r="J3" s="3">
         <v>13</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c t="s" r="K3" s="3">
         <v>14</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c t="s" r="L3" s="9">
         <v>15</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c t="s" r="M3" s="9">
         <v>16</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c t="s" r="N3" s="9">
         <v>17</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c t="s" r="O3" s="8">
         <v>18</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c t="s" r="P3" s="8">
         <v>19</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c t="s" r="Q3" s="8">
         <v>20</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c t="s" r="R3" s="9">
         <v>21</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c t="s" r="S3" s="9">
         <v>22</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c t="s" r="T3" s="9">
         <v>23</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c t="s" r="U3" s="8">
         <v>24</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c t="s" r="V3" s="11">
         <v>25</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c t="s" r="W3" s="10">
         <v>26</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c t="s" r="X3" s="11">
         <v>27</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c t="s" r="Y3" s="11">
         <v>28</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c t="s" r="Z3" s="5">
         <v>29</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c t="s" r="AA3" s="2">
         <v>30</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c t="s" r="AB3" s="2">
         <v>31</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c t="s" r="AC3" s="3">
         <v>32</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="4" spans="1:29">
-      <c r="A4" s="1" t="n"/>
-      <c r="B4" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="4">
+      <c t="n" r="A4" s="1"/>
+      <c t="s" r="B4">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>34</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c t="s" r="D4" s="14">
         <v>35</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c t="s" r="E4" s="12">
         <v>36</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c t="s" r="F4" s="13">
         <v>37</v>
       </c>
-      <c r="G4" s="1" t="n"/>
-      <c r="H4" s="1" t="n"/>
-      <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="n"/>
-      <c r="K4" s="14" t="s">
+      <c t="n" r="G4" s="1"/>
+      <c t="n" r="H4" s="1"/>
+      <c t="n" r="I4" s="1"/>
+      <c t="n" r="J4" s="1"/>
+      <c t="s" r="K4" s="14">
         <v>38</v>
       </c>
-      <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="n"/>
-      <c r="N4" s="1" t="n"/>
-      <c r="O4" s="1" t="n"/>
-      <c r="P4" s="1" t="n"/>
-      <c r="Q4" s="1" t="n"/>
-      <c r="R4" s="1" t="n"/>
-      <c r="S4" s="1" t="n"/>
-      <c r="T4" s="1" t="n"/>
-      <c r="U4" s="1" t="n"/>
-      <c r="V4" s="15" t="s">
+      <c t="n" r="L4" s="1"/>
+      <c t="n" r="M4" s="1"/>
+      <c t="n" r="N4" s="1"/>
+      <c t="n" r="O4" s="1"/>
+      <c t="n" r="P4" s="1"/>
+      <c t="n" r="Q4" s="1"/>
+      <c t="n" r="R4" s="1"/>
+      <c t="n" r="S4" s="1"/>
+      <c t="n" r="T4" s="1"/>
+      <c t="n" r="U4" s="1"/>
+      <c t="s" r="V4" s="15">
         <v>39</v>
       </c>
-      <c r="W4" s="1" t="n"/>
-      <c r="X4" s="1" t="s">
+      <c t="n" r="W4" s="1"/>
+      <c t="s" r="X4" s="1">
         <v>40</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c t="s" r="Y4" s="1">
         <v>41</v>
       </c>
-      <c r="Z4" s="1" t="n"/>
-      <c r="AA4" s="17" t="s">
+      <c t="n" r="Z4" s="1"/>
+      <c t="s" r="AA4" s="17">
         <v>42</v>
       </c>
-      <c r="AB4" t="n">
+      <c t="n" r="AB4">
         <v>16</v>
       </c>
-      <c r="AC4" s="16" t="s">
+      <c t="s" r="AC4" s="16">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="5" spans="1:29">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="5">
+      <c t="n" r="A5" s="1"/>
+      <c t="s" r="B5">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>45</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c t="s" r="D5" s="14">
         <v>35</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c t="s" r="E5" s="12">
         <v>36</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c t="s" r="F5" s="13">
         <v>37</v>
       </c>
-      <c r="G5" s="1" t="n"/>
-      <c r="H5" s="1" t="n"/>
-      <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
-      <c r="K5" s="14" t="s">
+      <c t="n" r="G5" s="1"/>
+      <c t="n" r="H5" s="1"/>
+      <c t="n" r="I5" s="1"/>
+      <c t="n" r="J5" s="1"/>
+      <c t="s" r="K5" s="14">
         <v>38</v>
       </c>
-      <c r="L5" s="1" t="n"/>
-      <c r="M5" s="1" t="n"/>
-      <c r="N5" s="1" t="n"/>
-      <c r="O5" s="1" t="n"/>
-      <c r="P5" s="1" t="n"/>
-      <c r="Q5" s="1" t="n"/>
-      <c r="R5" s="1" t="n"/>
-      <c r="S5" s="1" t="n"/>
-      <c r="T5" s="1" t="n"/>
-      <c r="U5" s="1" t="n"/>
-      <c r="V5" s="15" t="s">
+      <c t="n" r="L5" s="1"/>
+      <c t="n" r="M5" s="1"/>
+      <c t="n" r="N5" s="1"/>
+      <c t="n" r="O5" s="1"/>
+      <c t="n" r="P5" s="1"/>
+      <c t="n" r="Q5" s="1"/>
+      <c t="n" r="R5" s="1"/>
+      <c t="n" r="S5" s="1"/>
+      <c t="n" r="T5" s="1"/>
+      <c t="n" r="U5" s="1"/>
+      <c t="s" r="V5" s="15">
         <v>39</v>
       </c>
-      <c r="W5" s="1" t="n"/>
-      <c r="X5" s="1" t="s">
+      <c t="n" r="W5" s="1"/>
+      <c t="s" r="X5" s="1">
         <v>40</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c t="s" r="Y5" s="1">
         <v>41</v>
       </c>
-      <c r="Z5" s="1" t="n"/>
-      <c r="AA5" s="18" t="s">
+      <c t="n" r="Z5" s="1"/>
+      <c t="s" r="AA5" s="18">
         <v>42</v>
       </c>
-      <c r="AB5" t="n">
+      <c t="n" r="AB5">
         <v>64</v>
       </c>
-      <c r="AC5" s="16" t="s">
+      <c t="s" r="AC5" s="16">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="6" spans="1:29">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="6">
+      <c t="n" r="A6" s="1"/>
+      <c t="s" r="B6">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>47</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c t="s" r="D6" s="14">
         <v>35</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c t="s" r="E6" s="12">
         <v>36</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c t="s" r="F6" s="13">
         <v>37</v>
       </c>
-      <c r="G6" s="1" t="n"/>
-      <c r="H6" s="1" t="n"/>
-      <c r="I6" s="1" t="n"/>
-      <c r="J6" s="1" t="n"/>
-      <c r="K6" s="14" t="s">
+      <c t="n" r="G6" s="1"/>
+      <c t="n" r="H6" s="1"/>
+      <c t="n" r="I6" s="1"/>
+      <c t="n" r="J6" s="1"/>
+      <c t="s" r="K6" s="14">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="n"/>
-      <c r="M6" s="1" t="n"/>
-      <c r="N6" s="1" t="n"/>
-      <c r="O6" s="1" t="n"/>
-      <c r="P6" s="1" t="n"/>
-      <c r="Q6" s="1" t="n"/>
-      <c r="R6" s="1" t="n"/>
-      <c r="S6" s="1" t="n"/>
-      <c r="T6" s="1" t="n"/>
-      <c r="U6" s="1" t="n"/>
-      <c r="V6" s="15" t="s">
+      <c t="n" r="L6" s="1"/>
+      <c t="n" r="M6" s="1"/>
+      <c t="n" r="N6" s="1"/>
+      <c t="n" r="O6" s="1"/>
+      <c t="n" r="P6" s="1"/>
+      <c t="n" r="Q6" s="1"/>
+      <c t="n" r="R6" s="1"/>
+      <c t="n" r="S6" s="1"/>
+      <c t="n" r="T6" s="1"/>
+      <c t="n" r="U6" s="1"/>
+      <c t="s" r="V6" s="15">
         <v>39</v>
       </c>
-      <c r="W6" s="1" t="n"/>
-      <c r="X6" s="1" t="s">
+      <c t="n" r="W6" s="1"/>
+      <c t="s" r="X6" s="1">
         <v>40</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c t="s" r="Y6" s="1">
         <v>41</v>
       </c>
-      <c r="Z6" s="1" t="n"/>
-      <c r="AA6" s="19" t="s">
+      <c t="n" r="Z6" s="1"/>
+      <c t="s" r="AA6" s="19">
         <v>48</v>
       </c>
-      <c r="AB6" t="n">
+      <c t="n" r="AB6">
         <v>256</v>
       </c>
-      <c r="AC6" s="16" t="s">
+      <c t="s" r="AC6" s="16">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="7" spans="1:29">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="7">
+      <c t="n" r="A7" s="1"/>
+      <c t="s" r="B7">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>47</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c t="s" r="D7" s="14">
         <v>35</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c t="s" r="E7" s="12">
         <v>36</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c t="s" r="F7" s="13">
         <v>37</v>
       </c>
-      <c r="G7" s="1" t="n"/>
-      <c r="H7" s="1" t="n"/>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
-      <c r="K7" s="14" t="s">
+      <c t="n" r="G7" s="1"/>
+      <c t="n" r="H7" s="1"/>
+      <c t="n" r="I7" s="1"/>
+      <c t="n" r="J7" s="1"/>
+      <c t="s" r="K7" s="14">
         <v>38</v>
       </c>
-      <c r="L7" s="1" t="n"/>
-      <c r="M7" s="1" t="n"/>
-      <c r="N7" s="1" t="n"/>
-      <c r="O7" s="1" t="n"/>
-      <c r="P7" s="1" t="n"/>
-      <c r="Q7" s="1" t="n"/>
-      <c r="R7" s="1" t="n"/>
-      <c r="S7" s="1" t="n"/>
-      <c r="T7" s="1" t="n"/>
-      <c r="U7" s="1" t="n"/>
-      <c r="V7" s="15" t="s">
+      <c t="n" r="L7" s="1"/>
+      <c t="n" r="M7" s="1"/>
+      <c t="n" r="N7" s="1"/>
+      <c t="n" r="O7" s="1"/>
+      <c t="n" r="P7" s="1"/>
+      <c t="n" r="Q7" s="1"/>
+      <c t="n" r="R7" s="1"/>
+      <c t="n" r="S7" s="1"/>
+      <c t="n" r="T7" s="1"/>
+      <c t="n" r="U7" s="1"/>
+      <c t="s" r="V7" s="15">
         <v>39</v>
       </c>
-      <c r="W7" s="1" t="n"/>
-      <c r="X7" s="1" t="s">
+      <c t="n" r="W7" s="1"/>
+      <c t="s" r="X7" s="1">
         <v>40</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c t="s" r="Y7" s="1">
         <v>41</v>
       </c>
-      <c r="Z7" s="1" t="n"/>
-      <c r="AA7" s="19" t="s">
+      <c t="n" r="Z7" s="1"/>
+      <c t="s" r="AA7" s="19">
         <v>50</v>
       </c>
-      <c r="AB7" t="n">
+      <c t="n" r="AB7">
         <v>128</v>
       </c>
-      <c r="AC7" s="16" t="s">
+      <c t="s" r="AC7" s="16">
         <v>51</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="8" spans="1:29">
-      <c r="B8" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="8">
+      <c t="s" r="B8">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>47</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c t="s" r="D8" s="14">
         <v>35</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c t="s" r="E8" s="12">
         <v>36</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c t="s" r="F8" s="13">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="n"/>
-      <c r="K8" s="14" t="s">
+      <c t="n" r="G8" s="1"/>
+      <c t="s" r="K8" s="14">
         <v>38</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c t="s" r="V8" s="15">
         <v>39</v>
       </c>
-      <c r="W8" s="1" t="n"/>
-      <c r="X8" s="1" t="s">
+      <c t="n" r="W8" s="1"/>
+      <c t="s" r="X8" s="1">
         <v>40</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c t="s" r="Y8" s="1">
         <v>41</v>
       </c>
-      <c r="AA8" s="19" t="s">
+      <c t="s" r="AA8" s="19">
         <v>53</v>
       </c>
-      <c r="AB8" t="n">
+      <c t="n" r="AB8">
         <v>64</v>
       </c>
-      <c r="AC8" s="16" t="s">
+      <c t="s" r="AC8" s="16">
         <v>54</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="9" spans="1:29">
-      <c r="B9" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="9">
+      <c t="s" r="B9">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>34</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c t="s" r="D9" s="14">
         <v>35</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c t="s" r="E9" s="12">
         <v>36</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c t="s" r="F9" s="13">
         <v>37</v>
       </c>
-      <c r="G9" s="1" t="n"/>
-      <c r="K9" s="14" t="s">
+      <c t="n" r="G9" s="1"/>
+      <c t="s" r="K9" s="14">
         <v>38</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c t="s" r="V9" s="15">
         <v>39</v>
       </c>
-      <c r="W9" s="1" t="n"/>
-      <c r="X9" s="1" t="s">
+      <c t="n" r="W9" s="1"/>
+      <c t="s" r="X9" s="1">
         <v>40</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c t="s" r="Y9" s="1">
         <v>41</v>
       </c>
-      <c r="AA9" s="20" t="s">
+      <c t="s" r="AA9" s="20">
         <v>56</v>
       </c>
-      <c r="AB9" t="n">
+      <c t="n" r="AB9">
         <v>8</v>
       </c>
-      <c r="AC9" s="16" t="s">
+      <c t="s" r="AC9" s="16">
         <v>57</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="10" spans="1:29">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="10">
+      <c t="n" r="A10" s="1"/>
+      <c t="s" r="B10">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>59</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c t="s" r="D10" s="14">
         <v>35</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c t="s" r="E10" s="12">
         <v>36</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c t="s" r="F10" s="13">
         <v>37</v>
       </c>
-      <c r="G10" s="1" t="n"/>
-      <c r="H10" s="1" t="n"/>
-      <c r="I10" s="1" t="n"/>
-      <c r="J10" s="1" t="n"/>
-      <c r="K10" s="14" t="s">
+      <c t="n" r="G10" s="1"/>
+      <c t="n" r="H10" s="1"/>
+      <c t="n" r="I10" s="1"/>
+      <c t="n" r="J10" s="1"/>
+      <c t="s" r="K10" s="14">
         <v>38</v>
       </c>
-      <c r="L10" s="1" t="n"/>
-      <c r="M10" s="1" t="n"/>
-      <c r="N10" s="1" t="n"/>
-      <c r="O10" s="1" t="n"/>
-      <c r="P10" s="1" t="n"/>
-      <c r="Q10" s="1" t="n"/>
-      <c r="R10" s="1" t="n"/>
-      <c r="S10" s="1" t="n"/>
-      <c r="T10" s="1" t="n"/>
-      <c r="U10" s="1" t="n"/>
-      <c r="V10" s="15" t="s">
+      <c t="n" r="L10" s="1"/>
+      <c t="n" r="M10" s="1"/>
+      <c t="n" r="N10" s="1"/>
+      <c t="n" r="O10" s="1"/>
+      <c t="n" r="P10" s="1"/>
+      <c t="n" r="Q10" s="1"/>
+      <c t="n" r="R10" s="1"/>
+      <c t="n" r="S10" s="1"/>
+      <c t="n" r="T10" s="1"/>
+      <c t="n" r="U10" s="1"/>
+      <c t="s" r="V10" s="15">
         <v>39</v>
       </c>
-      <c r="W10" s="1" t="n"/>
-      <c r="X10" s="1" t="s">
+      <c t="n" r="W10" s="1"/>
+      <c t="s" r="X10" s="1">
         <v>40</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c t="s" r="Y10" s="1">
         <v>41</v>
       </c>
-      <c r="Z10" s="1" t="n"/>
-      <c r="AA10" s="21" t="s">
+      <c t="n" r="Z10" s="1"/>
+      <c t="s" r="AA10" s="21">
         <v>60</v>
       </c>
-      <c r="AB10" t="n">
+      <c t="n" r="AB10">
         <v>32</v>
       </c>
-      <c r="AC10" s="16" t="s">
+      <c t="s" r="AC10" s="16">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="11" spans="1:29">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="11">
+      <c t="n" r="A11" s="1"/>
+      <c t="s" r="B11">
         <v>61</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>62</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c t="s" r="D11" s="14">
         <v>35</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c t="s" r="E11" s="12">
         <v>36</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c t="s" r="F11" s="13">
         <v>37</v>
       </c>
-      <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
-      <c r="K11" s="14" t="s">
+      <c t="n" r="G11" s="1"/>
+      <c t="n" r="H11" s="1"/>
+      <c t="n" r="I11" s="1"/>
+      <c t="n" r="J11" s="1"/>
+      <c t="s" r="K11" s="14">
         <v>38</v>
       </c>
-      <c r="L11" s="1" t="n"/>
-      <c r="M11" s="1" t="n"/>
-      <c r="N11" s="1" t="n"/>
-      <c r="O11" s="1" t="n"/>
-      <c r="P11" s="1" t="n"/>
-      <c r="Q11" s="1" t="n"/>
-      <c r="R11" s="1" t="n"/>
-      <c r="S11" s="1" t="n"/>
-      <c r="T11" s="1" t="n"/>
-      <c r="U11" s="1" t="n"/>
-      <c r="V11" s="15" t="s">
+      <c t="n" r="L11" s="1"/>
+      <c t="n" r="M11" s="1"/>
+      <c t="n" r="N11" s="1"/>
+      <c t="n" r="O11" s="1"/>
+      <c t="n" r="P11" s="1"/>
+      <c t="n" r="Q11" s="1"/>
+      <c t="n" r="R11" s="1"/>
+      <c t="n" r="S11" s="1"/>
+      <c t="n" r="T11" s="1"/>
+      <c t="n" r="U11" s="1"/>
+      <c t="s" r="V11" s="15">
         <v>39</v>
       </c>
-      <c r="W11" s="1" t="n"/>
-      <c r="X11" s="1" t="s">
+      <c t="n" r="W11" s="1"/>
+      <c t="s" r="X11" s="1">
         <v>40</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c t="s" r="Y11" s="1">
         <v>41</v>
       </c>
-      <c r="Z11" s="1" t="n"/>
-      <c r="AA11" s="21" t="s">
+      <c t="n" r="Z11" s="1"/>
+      <c t="s" r="AA11" s="22">
         <v>63</v>
       </c>
-      <c r="AB11" t="n">
+      <c t="n" r="AB11">
         <v>8</v>
       </c>
-      <c r="AC11" s="16" t="s">
+      <c t="s" r="AC11" s="16">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="24" r="12" spans="1:29">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" t="s">
+    <row spans="1:29" customHeight="1" ht="24" r="12">
+      <c t="n" r="A12" s="1"/>
+      <c t="s" r="B12">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>62</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c t="s" r="D12" s="14">
         <v>35</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c t="s" r="E12" s="12">
         <v>36</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c t="s" r="F12" s="13">
         <v>37</v>
       </c>
-      <c r="G12" s="1" t="n"/>
-      <c r="H12" s="1" t="n"/>
-      <c r="I12" s="1" t="n"/>
-      <c r="J12" s="1" t="n"/>
-      <c r="K12" s="14" t="s">
+      <c t="n" r="G12" s="1"/>
+      <c t="n" r="H12" s="1"/>
+      <c t="n" r="I12" s="1"/>
+      <c t="n" r="J12" s="1"/>
+      <c t="s" r="K12" s="14">
         <v>38</v>
       </c>
-      <c r="L12" s="1" t="n"/>
-      <c r="M12" s="1" t="n"/>
-      <c r="N12" s="1" t="n"/>
-      <c r="O12" s="1" t="n"/>
-      <c r="P12" s="1" t="n"/>
-      <c r="Q12" s="1" t="n"/>
-      <c r="R12" s="1" t="n"/>
-      <c r="S12" s="1" t="n"/>
-      <c r="T12" s="1" t="n"/>
-      <c r="U12" s="1" t="n"/>
-      <c r="V12" s="15" t="s">
+      <c t="n" r="L12" s="1"/>
+      <c t="n" r="M12" s="1"/>
+      <c t="n" r="N12" s="1"/>
+      <c t="n" r="O12" s="1"/>
+      <c t="n" r="P12" s="1"/>
+      <c t="n" r="Q12" s="1"/>
+      <c t="n" r="R12" s="1"/>
+      <c t="n" r="S12" s="1"/>
+      <c t="n" r="T12" s="1"/>
+      <c t="n" r="U12" s="1"/>
+      <c t="s" r="V12" s="15">
         <v>39</v>
       </c>
-      <c r="W12" s="1" t="n"/>
-      <c r="X12" s="1" t="s">
+      <c t="n" r="W12" s="1"/>
+      <c t="s" r="X12" s="1">
         <v>40</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c t="s" r="Y12" s="1">
         <v>41</v>
       </c>
-      <c r="Z12" s="1" t="n"/>
-      <c r="AA12" s="21" t="n"/>
-      <c r="AB12" t="n">
+      <c t="n" r="Z12" s="1"/>
+      <c t="n" r="AA12" s="22"/>
+      <c t="n" r="AB12">
         <v>8</v>
       </c>
-      <c r="AC12" s="16" t="s">
+      <c t="s" r="AC12" s="16">
         <v>43</v>
       </c>
     </row>
@@ -1932,7 +1941,7 @@
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <legacyDrawing r:id="commentsvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -1950,503 +1959,503 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row spans="1:1" r="2">
+      <c t="s" r="A2">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row spans="1:1" r="3">
+      <c t="s" r="A3">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row spans="1:1" r="4">
+      <c t="s" r="A4">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row spans="1:1" r="5">
+      <c t="s" r="A5">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row spans="1:1" r="6">
+      <c t="s" r="A6">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row spans="1:1" r="7">
+      <c t="s" r="A7">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row spans="1:1" r="8">
+      <c t="s" r="A8">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row spans="1:1" r="9">
+      <c t="s" r="A9">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+    <row spans="1:1" r="10">
+      <c t="s" r="A10">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row spans="1:1" r="11">
+      <c t="s" r="A11">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+    <row spans="1:1" r="12">
+      <c t="s" r="A12">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+    <row spans="1:1" r="13">
+      <c t="s" r="A13">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row spans="1:1" r="14">
+      <c t="s" r="A14">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+    <row spans="1:1" r="15">
+      <c t="s" r="A15">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row spans="1:1" r="16">
+      <c t="s" r="A16">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row spans="1:1" r="17">
+      <c t="s" r="A17">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row spans="1:1" r="18">
+      <c t="s" r="A18">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row spans="1:1" r="20">
+      <c t="s" r="A20">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row spans="1:1" r="21">
+      <c t="s" r="A21">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row spans="1:1" r="22">
+      <c t="s" r="A22">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row spans="1:1" r="23">
+      <c t="s" r="A23">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row spans="1:1" r="24">
+      <c t="s" r="A24">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row spans="1:1" r="25">
+      <c t="s" r="A25">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row spans="1:1" r="26">
+      <c t="s" r="A26">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+    <row spans="1:1" r="27">
+      <c t="s" r="A27">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+    <row spans="1:1" r="28">
+      <c t="s" r="A28">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+    <row spans="1:1" r="29">
+      <c t="s" r="A29">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row spans="1:1" r="30">
+      <c t="s" r="A30">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+    <row spans="1:1" r="31">
+      <c t="s" r="A31">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+    <row spans="1:1" r="32">
+      <c t="s" r="A32">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row spans="1:1" r="33">
+      <c t="s" r="A33">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row spans="1:1" r="34">
+      <c t="s" r="A34">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
+    <row spans="1:1" r="35">
+      <c t="s" r="A35">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+    <row spans="1:1" r="36">
+      <c t="s" r="A36">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
+    <row spans="1:1" r="37">
+      <c t="s" r="A37">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row spans="1:1" r="38">
+      <c t="s" r="A38">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+    <row spans="1:1" r="39">
+      <c t="s" r="A39">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
+    <row spans="1:1" r="40">
+      <c t="s" r="A40">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
+    <row spans="1:1" r="41">
+      <c t="s" r="A41">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
+    <row spans="1:1" r="42">
+      <c t="s" r="A42">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
+    <row spans="1:1" r="43">
+      <c t="s" r="A43">
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
+    <row spans="1:1" r="44">
+      <c t="s" r="A44">
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
+    <row spans="1:1" r="45">
+      <c t="s" r="A45">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+    <row spans="1:1" r="46">
+      <c t="s" r="A46">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
+    <row spans="1:1" r="47">
+      <c t="s" r="A47">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
+    <row spans="1:1" r="48">
+      <c t="s" r="A48">
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
+    <row spans="1:1" r="49">
+      <c t="s" r="A49">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
+    <row spans="1:1" r="50">
+      <c t="s" r="A50">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
+    <row spans="1:1" r="51">
+      <c t="s" r="A51">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
+    <row spans="1:1" r="52">
+      <c t="s" r="A52">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
+    <row spans="1:1" r="53">
+      <c t="s" r="A53">
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row spans="1:1" r="54">
+      <c t="s" r="A54">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row spans="1:1" r="55">
+      <c t="s" r="A55">
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
+    <row spans="1:1" r="56">
+      <c t="s" r="A56">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    <row spans="1:1" r="57">
+      <c t="s" r="A57">
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
+    <row spans="1:1" r="58">
+      <c t="s" r="A58">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
+    <row spans="1:1" r="59">
+      <c t="s" r="A59">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
+    <row spans="1:1" r="60">
+      <c t="s" r="A60">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
+    <row spans="1:1" r="61">
+      <c t="s" r="A61">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
+    <row spans="1:1" r="62">
+      <c t="s" r="A62">
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
+    <row spans="1:1" r="64">
+      <c t="s" r="A64">
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+    <row spans="1:1" r="65">
+      <c t="s" r="A65">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
+    <row spans="1:1" r="66">
+      <c t="s" r="A66">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
+    <row spans="1:1" r="67">
+      <c t="s" r="A67">
         <v>124</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+    <row spans="1:1" r="68">
+      <c t="s" r="A68">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+    <row spans="1:1" r="69">
+      <c t="s" r="A69">
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+    <row spans="1:1" r="70">
+      <c t="s" r="A70">
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+    <row spans="1:1" r="71">
+      <c t="s" r="A71">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
+    <row spans="1:1" r="72">
+      <c t="s" r="A72">
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+    <row spans="1:1" r="73">
+      <c t="s" r="A73">
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+    <row spans="1:1" r="74">
+      <c t="s" r="A74">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+    <row spans="1:1" r="76">
+      <c t="s" r="A76">
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
+    <row spans="1:1" r="77">
+      <c t="s" r="A77">
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
+    <row spans="1:1" r="78">
+      <c t="s" r="A78">
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
+    <row spans="1:1" r="79">
+      <c t="s" r="A79">
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
+    <row spans="1:1" r="80">
+      <c t="s" r="A80">
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
+    <row spans="1:1" r="81">
+      <c t="s" r="A81">
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
+    <row spans="1:1" r="82">
+      <c t="s" r="A82">
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
+    <row spans="1:1" r="83">
+      <c t="s" r="A83">
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
+    <row spans="1:1" r="84">
+      <c t="s" r="A84">
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
+    <row spans="1:1" r="85">
+      <c t="s" r="A85">
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
+    <row spans="1:1" r="86">
+      <c t="s" r="A86">
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
+    <row spans="1:1" r="87">
+      <c t="s" r="A87">
         <v>142</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
+    <row spans="1:1" r="88">
+      <c t="s" r="A88">
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
+    <row spans="1:1" r="89">
+      <c t="s" r="A89">
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
+    <row spans="1:1" r="90">
+      <c t="s" r="A90">
         <v>145</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
+    <row spans="1:1" r="91">
+      <c t="s" r="A91">
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
+    <row spans="1:1" r="92">
+      <c t="s" r="A92">
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
+    <row spans="1:1" r="93">
+      <c t="s" r="A93">
         <v>147</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
+    <row spans="1:1" r="94">
+      <c t="s" r="A94">
         <v>148</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
+    <row spans="1:1" r="95">
+      <c t="s" r="A95">
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
+    <row spans="1:1" r="96">
+      <c t="s" r="A96">
         <v>150</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+    <row spans="1:1" r="97">
+      <c t="s" r="A97">
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
+    <row spans="1:1" r="98">
+      <c t="s" r="A98">
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
+    <row spans="1:1" r="99">
+      <c t="s" r="A99">
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
+    <row spans="1:1" r="100">
+      <c t="s" r="A100">
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
+    <row spans="1:1" r="101">
+      <c t="s" r="A101">
         <v>155</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
+    <row spans="1:1" r="102">
+      <c t="s" r="A102">
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
+    <row spans="1:1" r="103">
+      <c t="s" r="A103">
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+    <row spans="1:1" r="104">
+      <c t="s" r="A104">
         <v>158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update example result file
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -198,17 +198,17 @@
     </comment>
     <comment authorId="1" ref="AA10" shapeId="0">
       <text>
-        <t>Not a virus</t>
+        <t>Not the name of virus</t>
       </text>
     </comment>
     <comment authorId="1" ref="AA11" shapeId="0">
       <text>
-        <t>Not found in NCBI Taxonomy`</t>
+        <t>Not found in NCBI Taxonomy</t>
       </text>
     </comment>
     <comment authorId="1" ref="AA12" shapeId="0">
       <text>
-        <t>Not found in NCBI Taxonomy`</t>
+        <t>Not found in NCBI Taxonomy</t>
       </text>
     </comment>
   </commentList>
@@ -917,9 +917,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -989,9 +989,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -1349,571 +1349,571 @@
     <col customWidth="1" max="29" min="28" width="13.5"/>
   </cols>
   <sheetData>
-    <row spans="1:29" customHeight="1" ht="38.25" r="1">
-      <c t="s" r="A1" s="2">
+    <row spans="1:29" ht="38.25" customHeight="1" r="1">
+      <c t="s" s="2" r="A1">
         <v>0</v>
       </c>
-      <c t="s" r="B1" s="2">
+      <c t="s" s="2" r="B1">
         <v>1</v>
       </c>
-      <c t="s" r="C1" s="2">
+      <c t="s" s="2" r="C1">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="51" r="2">
-      <c t="s" r="A2" s="1">
+    <row spans="1:29" ht="51" customHeight="1" r="2">
+      <c t="s" s="1" r="A2">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="63.75" r="3">
-      <c t="s" r="A3" s="4">
+    <row spans="1:29" ht="63.75" customHeight="1" r="3">
+      <c t="s" s="4" r="A3">
         <v>4</v>
       </c>
-      <c t="s" r="B3" s="7">
+      <c t="s" s="7" r="B3">
         <v>5</v>
       </c>
-      <c t="s" r="C3" s="9">
+      <c t="s" s="9" r="C3">
         <v>6</v>
       </c>
-      <c t="s" r="D3" s="11">
+      <c t="s" s="11" r="D3">
         <v>7</v>
       </c>
-      <c t="s" r="E3" s="7">
+      <c t="s" s="7" r="E3">
         <v>8</v>
       </c>
-      <c t="s" r="F3" s="7">
+      <c t="s" s="7" r="F3">
         <v>9</v>
       </c>
-      <c t="s" r="G3" s="6">
+      <c t="s" s="6" r="G3">
         <v>10</v>
       </c>
-      <c t="s" r="H3" s="6">
+      <c t="s" s="6" r="H3">
         <v>11</v>
       </c>
-      <c t="s" r="I3" s="6">
+      <c t="s" s="6" r="I3">
         <v>12</v>
       </c>
-      <c t="s" r="J3" s="3">
+      <c t="s" s="3" r="J3">
         <v>13</v>
       </c>
-      <c t="s" r="K3" s="3">
+      <c t="s" s="3" r="K3">
         <v>14</v>
       </c>
-      <c t="s" r="L3" s="9">
+      <c t="s" s="9" r="L3">
         <v>15</v>
       </c>
-      <c t="s" r="M3" s="9">
+      <c t="s" s="9" r="M3">
         <v>16</v>
       </c>
-      <c t="s" r="N3" s="9">
+      <c t="s" s="9" r="N3">
         <v>17</v>
       </c>
-      <c t="s" r="O3" s="8">
+      <c t="s" s="8" r="O3">
         <v>18</v>
       </c>
-      <c t="s" r="P3" s="8">
+      <c t="s" s="8" r="P3">
         <v>19</v>
       </c>
-      <c t="s" r="Q3" s="8">
+      <c t="s" s="8" r="Q3">
         <v>20</v>
       </c>
-      <c t="s" r="R3" s="9">
+      <c t="s" s="9" r="R3">
         <v>21</v>
       </c>
-      <c t="s" r="S3" s="9">
+      <c t="s" s="9" r="S3">
         <v>22</v>
       </c>
-      <c t="s" r="T3" s="9">
+      <c t="s" s="9" r="T3">
         <v>23</v>
       </c>
-      <c t="s" r="U3" s="8">
+      <c t="s" s="8" r="U3">
         <v>24</v>
       </c>
-      <c t="s" r="V3" s="11">
+      <c t="s" s="11" r="V3">
         <v>25</v>
       </c>
-      <c t="s" r="W3" s="10">
+      <c t="s" s="10" r="W3">
         <v>26</v>
       </c>
-      <c t="s" r="X3" s="11">
+      <c t="s" s="11" r="X3">
         <v>27</v>
       </c>
-      <c t="s" r="Y3" s="11">
+      <c t="s" s="11" r="Y3">
         <v>28</v>
       </c>
-      <c t="s" r="Z3" s="5">
+      <c t="s" s="5" r="Z3">
         <v>29</v>
       </c>
-      <c t="s" r="AA3" s="2">
+      <c t="s" s="2" r="AA3">
         <v>30</v>
       </c>
-      <c t="s" r="AB3" s="2">
+      <c t="s" s="2" r="AB3">
         <v>31</v>
       </c>
-      <c t="s" r="AC3" s="3">
+      <c t="s" s="3" r="AC3">
         <v>32</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="4">
-      <c t="n" r="A4" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="4">
+      <c t="n" s="1" r="A4"/>
       <c t="s" r="B4">
         <v>33</v>
       </c>
       <c t="s" r="C4">
         <v>34</v>
       </c>
-      <c t="s" r="D4" s="14">
+      <c t="s" s="14" r="D4">
         <v>35</v>
       </c>
-      <c t="s" r="E4" s="12">
+      <c t="s" s="12" r="E4">
         <v>36</v>
       </c>
-      <c t="s" r="F4" s="13">
+      <c t="s" s="13" r="F4">
         <v>37</v>
       </c>
-      <c t="n" r="G4" s="1"/>
-      <c t="n" r="H4" s="1"/>
-      <c t="n" r="I4" s="1"/>
-      <c t="n" r="J4" s="1"/>
-      <c t="s" r="K4" s="14">
+      <c t="n" s="1" r="G4"/>
+      <c t="n" s="1" r="H4"/>
+      <c t="n" s="1" r="I4"/>
+      <c t="n" s="1" r="J4"/>
+      <c t="s" s="14" r="K4">
         <v>38</v>
       </c>
-      <c t="n" r="L4" s="1"/>
-      <c t="n" r="M4" s="1"/>
-      <c t="n" r="N4" s="1"/>
-      <c t="n" r="O4" s="1"/>
-      <c t="n" r="P4" s="1"/>
-      <c t="n" r="Q4" s="1"/>
-      <c t="n" r="R4" s="1"/>
-      <c t="n" r="S4" s="1"/>
-      <c t="n" r="T4" s="1"/>
-      <c t="n" r="U4" s="1"/>
-      <c t="s" r="V4" s="15">
+      <c t="n" s="1" r="L4"/>
+      <c t="n" s="1" r="M4"/>
+      <c t="n" s="1" r="N4"/>
+      <c t="n" s="1" r="O4"/>
+      <c t="n" s="1" r="P4"/>
+      <c t="n" s="1" r="Q4"/>
+      <c t="n" s="1" r="R4"/>
+      <c t="n" s="1" r="S4"/>
+      <c t="n" s="1" r="T4"/>
+      <c t="n" s="1" r="U4"/>
+      <c t="s" s="15" r="V4">
         <v>39</v>
       </c>
-      <c t="n" r="W4" s="1"/>
-      <c t="s" r="X4" s="1">
+      <c t="n" s="1" r="W4"/>
+      <c t="s" s="1" r="X4">
         <v>40</v>
       </c>
-      <c t="s" r="Y4" s="1">
+      <c t="s" s="1" r="Y4">
         <v>41</v>
       </c>
-      <c t="n" r="Z4" s="1"/>
-      <c t="s" r="AA4" s="17">
+      <c t="n" s="1" r="Z4"/>
+      <c t="s" s="17" r="AA4">
         <v>42</v>
       </c>
       <c t="n" r="AB4">
         <v>16</v>
       </c>
-      <c t="s" r="AC4" s="16">
+      <c t="s" s="16" r="AC4">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="5">
-      <c t="n" r="A5" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="5">
+      <c t="n" s="1" r="A5"/>
       <c t="s" r="B5">
         <v>44</v>
       </c>
       <c t="s" r="C5">
         <v>45</v>
       </c>
-      <c t="s" r="D5" s="14">
+      <c t="s" s="14" r="D5">
         <v>35</v>
       </c>
-      <c t="s" r="E5" s="12">
+      <c t="s" s="12" r="E5">
         <v>36</v>
       </c>
-      <c t="s" r="F5" s="13">
+      <c t="s" s="13" r="F5">
         <v>37</v>
       </c>
-      <c t="n" r="G5" s="1"/>
-      <c t="n" r="H5" s="1"/>
-      <c t="n" r="I5" s="1"/>
-      <c t="n" r="J5" s="1"/>
-      <c t="s" r="K5" s="14">
+      <c t="n" s="1" r="G5"/>
+      <c t="n" s="1" r="H5"/>
+      <c t="n" s="1" r="I5"/>
+      <c t="n" s="1" r="J5"/>
+      <c t="s" s="14" r="K5">
         <v>38</v>
       </c>
-      <c t="n" r="L5" s="1"/>
-      <c t="n" r="M5" s="1"/>
-      <c t="n" r="N5" s="1"/>
-      <c t="n" r="O5" s="1"/>
-      <c t="n" r="P5" s="1"/>
-      <c t="n" r="Q5" s="1"/>
-      <c t="n" r="R5" s="1"/>
-      <c t="n" r="S5" s="1"/>
-      <c t="n" r="T5" s="1"/>
-      <c t="n" r="U5" s="1"/>
-      <c t="s" r="V5" s="15">
+      <c t="n" s="1" r="L5"/>
+      <c t="n" s="1" r="M5"/>
+      <c t="n" s="1" r="N5"/>
+      <c t="n" s="1" r="O5"/>
+      <c t="n" s="1" r="P5"/>
+      <c t="n" s="1" r="Q5"/>
+      <c t="n" s="1" r="R5"/>
+      <c t="n" s="1" r="S5"/>
+      <c t="n" s="1" r="T5"/>
+      <c t="n" s="1" r="U5"/>
+      <c t="s" s="15" r="V5">
         <v>39</v>
       </c>
-      <c t="n" r="W5" s="1"/>
-      <c t="s" r="X5" s="1">
+      <c t="n" s="1" r="W5"/>
+      <c t="s" s="1" r="X5">
         <v>40</v>
       </c>
-      <c t="s" r="Y5" s="1">
+      <c t="s" s="1" r="Y5">
         <v>41</v>
       </c>
-      <c t="n" r="Z5" s="1"/>
-      <c t="s" r="AA5" s="18">
+      <c t="n" s="1" r="Z5"/>
+      <c t="s" s="18" r="AA5">
         <v>42</v>
       </c>
       <c t="n" r="AB5">
         <v>64</v>
       </c>
-      <c t="s" r="AC5" s="16">
+      <c t="s" s="16" r="AC5">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="6">
-      <c t="n" r="A6" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="6">
+      <c t="n" s="1" r="A6"/>
       <c t="s" r="B6">
         <v>46</v>
       </c>
       <c t="s" r="C6">
         <v>47</v>
       </c>
-      <c t="s" r="D6" s="14">
+      <c t="s" s="14" r="D6">
         <v>35</v>
       </c>
-      <c t="s" r="E6" s="12">
+      <c t="s" s="12" r="E6">
         <v>36</v>
       </c>
-      <c t="s" r="F6" s="13">
+      <c t="s" s="13" r="F6">
         <v>37</v>
       </c>
-      <c t="n" r="G6" s="1"/>
-      <c t="n" r="H6" s="1"/>
-      <c t="n" r="I6" s="1"/>
-      <c t="n" r="J6" s="1"/>
-      <c t="s" r="K6" s="14">
+      <c t="n" s="1" r="G6"/>
+      <c t="n" s="1" r="H6"/>
+      <c t="n" s="1" r="I6"/>
+      <c t="n" s="1" r="J6"/>
+      <c t="s" s="14" r="K6">
         <v>38</v>
       </c>
-      <c t="n" r="L6" s="1"/>
-      <c t="n" r="M6" s="1"/>
-      <c t="n" r="N6" s="1"/>
-      <c t="n" r="O6" s="1"/>
-      <c t="n" r="P6" s="1"/>
-      <c t="n" r="Q6" s="1"/>
-      <c t="n" r="R6" s="1"/>
-      <c t="n" r="S6" s="1"/>
-      <c t="n" r="T6" s="1"/>
-      <c t="n" r="U6" s="1"/>
-      <c t="s" r="V6" s="15">
+      <c t="n" s="1" r="L6"/>
+      <c t="n" s="1" r="M6"/>
+      <c t="n" s="1" r="N6"/>
+      <c t="n" s="1" r="O6"/>
+      <c t="n" s="1" r="P6"/>
+      <c t="n" s="1" r="Q6"/>
+      <c t="n" s="1" r="R6"/>
+      <c t="n" s="1" r="S6"/>
+      <c t="n" s="1" r="T6"/>
+      <c t="n" s="1" r="U6"/>
+      <c t="s" s="15" r="V6">
         <v>39</v>
       </c>
-      <c t="n" r="W6" s="1"/>
-      <c t="s" r="X6" s="1">
+      <c t="n" s="1" r="W6"/>
+      <c t="s" s="1" r="X6">
         <v>40</v>
       </c>
-      <c t="s" r="Y6" s="1">
+      <c t="s" s="1" r="Y6">
         <v>41</v>
       </c>
-      <c t="n" r="Z6" s="1"/>
-      <c t="s" r="AA6" s="19">
+      <c t="n" s="1" r="Z6"/>
+      <c t="s" s="19" r="AA6">
         <v>48</v>
       </c>
       <c t="n" r="AB6">
         <v>256</v>
       </c>
-      <c t="s" r="AC6" s="16">
+      <c t="s" s="16" r="AC6">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="7">
-      <c t="n" r="A7" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="7">
+      <c t="n" s="1" r="A7"/>
       <c t="s" r="B7">
         <v>49</v>
       </c>
       <c t="s" r="C7">
         <v>47</v>
       </c>
-      <c t="s" r="D7" s="14">
+      <c t="s" s="14" r="D7">
         <v>35</v>
       </c>
-      <c t="s" r="E7" s="12">
+      <c t="s" s="12" r="E7">
         <v>36</v>
       </c>
-      <c t="s" r="F7" s="13">
+      <c t="s" s="13" r="F7">
         <v>37</v>
       </c>
-      <c t="n" r="G7" s="1"/>
-      <c t="n" r="H7" s="1"/>
-      <c t="n" r="I7" s="1"/>
-      <c t="n" r="J7" s="1"/>
-      <c t="s" r="K7" s="14">
+      <c t="n" s="1" r="G7"/>
+      <c t="n" s="1" r="H7"/>
+      <c t="n" s="1" r="I7"/>
+      <c t="n" s="1" r="J7"/>
+      <c t="s" s="14" r="K7">
         <v>38</v>
       </c>
-      <c t="n" r="L7" s="1"/>
-      <c t="n" r="M7" s="1"/>
-      <c t="n" r="N7" s="1"/>
-      <c t="n" r="O7" s="1"/>
-      <c t="n" r="P7" s="1"/>
-      <c t="n" r="Q7" s="1"/>
-      <c t="n" r="R7" s="1"/>
-      <c t="n" r="S7" s="1"/>
-      <c t="n" r="T7" s="1"/>
-      <c t="n" r="U7" s="1"/>
-      <c t="s" r="V7" s="15">
+      <c t="n" s="1" r="L7"/>
+      <c t="n" s="1" r="M7"/>
+      <c t="n" s="1" r="N7"/>
+      <c t="n" s="1" r="O7"/>
+      <c t="n" s="1" r="P7"/>
+      <c t="n" s="1" r="Q7"/>
+      <c t="n" s="1" r="R7"/>
+      <c t="n" s="1" r="S7"/>
+      <c t="n" s="1" r="T7"/>
+      <c t="n" s="1" r="U7"/>
+      <c t="s" s="15" r="V7">
         <v>39</v>
       </c>
-      <c t="n" r="W7" s="1"/>
-      <c t="s" r="X7" s="1">
+      <c t="n" s="1" r="W7"/>
+      <c t="s" s="1" r="X7">
         <v>40</v>
       </c>
-      <c t="s" r="Y7" s="1">
+      <c t="s" s="1" r="Y7">
         <v>41</v>
       </c>
-      <c t="n" r="Z7" s="1"/>
-      <c t="s" r="AA7" s="19">
+      <c t="n" s="1" r="Z7"/>
+      <c t="s" s="19" r="AA7">
         <v>50</v>
       </c>
       <c t="n" r="AB7">
         <v>128</v>
       </c>
-      <c t="s" r="AC7" s="16">
+      <c t="s" s="16" r="AC7">
         <v>51</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="8">
+    <row spans="1:29" ht="24" customHeight="1" r="8">
       <c t="s" r="B8">
         <v>52</v>
       </c>
       <c t="s" r="C8">
         <v>47</v>
       </c>
-      <c t="s" r="D8" s="14">
+      <c t="s" s="14" r="D8">
         <v>35</v>
       </c>
-      <c t="s" r="E8" s="12">
+      <c t="s" s="12" r="E8">
         <v>36</v>
       </c>
-      <c t="s" r="F8" s="13">
+      <c t="s" s="13" r="F8">
         <v>37</v>
       </c>
-      <c t="n" r="G8" s="1"/>
-      <c t="s" r="K8" s="14">
+      <c t="n" s="1" r="G8"/>
+      <c t="s" s="14" r="K8">
         <v>38</v>
       </c>
-      <c t="s" r="V8" s="15">
+      <c t="s" s="15" r="V8">
         <v>39</v>
       </c>
-      <c t="n" r="W8" s="1"/>
-      <c t="s" r="X8" s="1">
+      <c t="n" s="1" r="W8"/>
+      <c t="s" s="1" r="X8">
         <v>40</v>
       </c>
-      <c t="s" r="Y8" s="1">
+      <c t="s" s="1" r="Y8">
         <v>41</v>
       </c>
-      <c t="s" r="AA8" s="19">
+      <c t="s" s="19" r="AA8">
         <v>53</v>
       </c>
       <c t="n" r="AB8">
         <v>64</v>
       </c>
-      <c t="s" r="AC8" s="16">
+      <c t="s" s="16" r="AC8">
         <v>54</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="9">
+    <row spans="1:29" ht="24" customHeight="1" r="9">
       <c t="s" r="B9">
         <v>55</v>
       </c>
       <c t="s" r="C9">
         <v>34</v>
       </c>
-      <c t="s" r="D9" s="14">
+      <c t="s" s="14" r="D9">
         <v>35</v>
       </c>
-      <c t="s" r="E9" s="12">
+      <c t="s" s="12" r="E9">
         <v>36</v>
       </c>
-      <c t="s" r="F9" s="13">
+      <c t="s" s="13" r="F9">
         <v>37</v>
       </c>
-      <c t="n" r="G9" s="1"/>
-      <c t="s" r="K9" s="14">
+      <c t="n" s="1" r="G9"/>
+      <c t="s" s="14" r="K9">
         <v>38</v>
       </c>
-      <c t="s" r="V9" s="15">
+      <c t="s" s="15" r="V9">
         <v>39</v>
       </c>
-      <c t="n" r="W9" s="1"/>
-      <c t="s" r="X9" s="1">
+      <c t="n" s="1" r="W9"/>
+      <c t="s" s="1" r="X9">
         <v>40</v>
       </c>
-      <c t="s" r="Y9" s="1">
+      <c t="s" s="1" r="Y9">
         <v>41</v>
       </c>
-      <c t="s" r="AA9" s="20">
+      <c t="s" s="20" r="AA9">
         <v>56</v>
       </c>
       <c t="n" r="AB9">
         <v>8</v>
       </c>
-      <c t="s" r="AC9" s="16">
+      <c t="s" s="16" r="AC9">
         <v>57</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="10">
-      <c t="n" r="A10" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="10">
+      <c t="n" s="1" r="A10"/>
       <c t="s" r="B10">
         <v>58</v>
       </c>
       <c t="s" r="C10">
         <v>59</v>
       </c>
-      <c t="s" r="D10" s="14">
+      <c t="s" s="14" r="D10">
         <v>35</v>
       </c>
-      <c t="s" r="E10" s="12">
+      <c t="s" s="12" r="E10">
         <v>36</v>
       </c>
-      <c t="s" r="F10" s="13">
+      <c t="s" s="13" r="F10">
         <v>37</v>
       </c>
-      <c t="n" r="G10" s="1"/>
-      <c t="n" r="H10" s="1"/>
-      <c t="n" r="I10" s="1"/>
-      <c t="n" r="J10" s="1"/>
-      <c t="s" r="K10" s="14">
+      <c t="n" s="1" r="G10"/>
+      <c t="n" s="1" r="H10"/>
+      <c t="n" s="1" r="I10"/>
+      <c t="n" s="1" r="J10"/>
+      <c t="s" s="14" r="K10">
         <v>38</v>
       </c>
-      <c t="n" r="L10" s="1"/>
-      <c t="n" r="M10" s="1"/>
-      <c t="n" r="N10" s="1"/>
-      <c t="n" r="O10" s="1"/>
-      <c t="n" r="P10" s="1"/>
-      <c t="n" r="Q10" s="1"/>
-      <c t="n" r="R10" s="1"/>
-      <c t="n" r="S10" s="1"/>
-      <c t="n" r="T10" s="1"/>
-      <c t="n" r="U10" s="1"/>
-      <c t="s" r="V10" s="15">
+      <c t="n" s="1" r="L10"/>
+      <c t="n" s="1" r="M10"/>
+      <c t="n" s="1" r="N10"/>
+      <c t="n" s="1" r="O10"/>
+      <c t="n" s="1" r="P10"/>
+      <c t="n" s="1" r="Q10"/>
+      <c t="n" s="1" r="R10"/>
+      <c t="n" s="1" r="S10"/>
+      <c t="n" s="1" r="T10"/>
+      <c t="n" s="1" r="U10"/>
+      <c t="s" s="15" r="V10">
         <v>39</v>
       </c>
-      <c t="n" r="W10" s="1"/>
-      <c t="s" r="X10" s="1">
+      <c t="n" s="1" r="W10"/>
+      <c t="s" s="1" r="X10">
         <v>40</v>
       </c>
-      <c t="s" r="Y10" s="1">
+      <c t="s" s="1" r="Y10">
         <v>41</v>
       </c>
-      <c t="n" r="Z10" s="1"/>
-      <c t="s" r="AA10" s="21">
+      <c t="n" s="1" r="Z10"/>
+      <c t="s" s="21" r="AA10">
         <v>60</v>
       </c>
       <c t="n" r="AB10">
         <v>32</v>
       </c>
-      <c t="s" r="AC10" s="16">
+      <c t="s" s="16" r="AC10">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="11">
-      <c t="n" r="A11" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="11">
+      <c t="n" s="1" r="A11"/>
       <c t="s" r="B11">
         <v>61</v>
       </c>
       <c t="s" r="C11">
         <v>62</v>
       </c>
-      <c t="s" r="D11" s="14">
+      <c t="s" s="14" r="D11">
         <v>35</v>
       </c>
-      <c t="s" r="E11" s="12">
+      <c t="s" s="12" r="E11">
         <v>36</v>
       </c>
-      <c t="s" r="F11" s="13">
+      <c t="s" s="13" r="F11">
         <v>37</v>
       </c>
-      <c t="n" r="G11" s="1"/>
-      <c t="n" r="H11" s="1"/>
-      <c t="n" r="I11" s="1"/>
-      <c t="n" r="J11" s="1"/>
-      <c t="s" r="K11" s="14">
+      <c t="n" s="1" r="G11"/>
+      <c t="n" s="1" r="H11"/>
+      <c t="n" s="1" r="I11"/>
+      <c t="n" s="1" r="J11"/>
+      <c t="s" s="14" r="K11">
         <v>38</v>
       </c>
-      <c t="n" r="L11" s="1"/>
-      <c t="n" r="M11" s="1"/>
-      <c t="n" r="N11" s="1"/>
-      <c t="n" r="O11" s="1"/>
-      <c t="n" r="P11" s="1"/>
-      <c t="n" r="Q11" s="1"/>
-      <c t="n" r="R11" s="1"/>
-      <c t="n" r="S11" s="1"/>
-      <c t="n" r="T11" s="1"/>
-      <c t="n" r="U11" s="1"/>
-      <c t="s" r="V11" s="15">
+      <c t="n" s="1" r="L11"/>
+      <c t="n" s="1" r="M11"/>
+      <c t="n" s="1" r="N11"/>
+      <c t="n" s="1" r="O11"/>
+      <c t="n" s="1" r="P11"/>
+      <c t="n" s="1" r="Q11"/>
+      <c t="n" s="1" r="R11"/>
+      <c t="n" s="1" r="S11"/>
+      <c t="n" s="1" r="T11"/>
+      <c t="n" s="1" r="U11"/>
+      <c t="s" s="15" r="V11">
         <v>39</v>
       </c>
-      <c t="n" r="W11" s="1"/>
-      <c t="s" r="X11" s="1">
+      <c t="n" s="1" r="W11"/>
+      <c t="s" s="1" r="X11">
         <v>40</v>
       </c>
-      <c t="s" r="Y11" s="1">
+      <c t="s" s="1" r="Y11">
         <v>41</v>
       </c>
-      <c t="n" r="Z11" s="1"/>
-      <c t="s" r="AA11" s="22">
+      <c t="n" s="1" r="Z11"/>
+      <c t="s" s="22" r="AA11">
         <v>63</v>
       </c>
       <c t="n" r="AB11">
         <v>8</v>
       </c>
-      <c t="s" r="AC11" s="16">
+      <c t="s" s="16" r="AC11">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" customHeight="1" ht="24" r="12">
-      <c t="n" r="A12" s="1"/>
+    <row spans="1:29" ht="24" customHeight="1" r="12">
+      <c t="n" s="1" r="A12"/>
       <c t="s" r="B12">
         <v>61</v>
       </c>
       <c t="s" r="C12">
         <v>62</v>
       </c>
-      <c t="s" r="D12" s="14">
+      <c t="s" s="14" r="D12">
         <v>35</v>
       </c>
-      <c t="s" r="E12" s="12">
+      <c t="s" s="12" r="E12">
         <v>36</v>
       </c>
-      <c t="s" r="F12" s="13">
+      <c t="s" s="13" r="F12">
         <v>37</v>
       </c>
-      <c t="n" r="G12" s="1"/>
-      <c t="n" r="H12" s="1"/>
-      <c t="n" r="I12" s="1"/>
-      <c t="n" r="J12" s="1"/>
-      <c t="s" r="K12" s="14">
+      <c t="n" s="1" r="G12"/>
+      <c t="n" s="1" r="H12"/>
+      <c t="n" s="1" r="I12"/>
+      <c t="n" s="1" r="J12"/>
+      <c t="s" s="14" r="K12">
         <v>38</v>
       </c>
-      <c t="n" r="L12" s="1"/>
-      <c t="n" r="M12" s="1"/>
-      <c t="n" r="N12" s="1"/>
-      <c t="n" r="O12" s="1"/>
-      <c t="n" r="P12" s="1"/>
-      <c t="n" r="Q12" s="1"/>
-      <c t="n" r="R12" s="1"/>
-      <c t="n" r="S12" s="1"/>
-      <c t="n" r="T12" s="1"/>
-      <c t="n" r="U12" s="1"/>
-      <c t="s" r="V12" s="15">
+      <c t="n" s="1" r="L12"/>
+      <c t="n" s="1" r="M12"/>
+      <c t="n" s="1" r="N12"/>
+      <c t="n" s="1" r="O12"/>
+      <c t="n" s="1" r="P12"/>
+      <c t="n" s="1" r="Q12"/>
+      <c t="n" s="1" r="R12"/>
+      <c t="n" s="1" r="S12"/>
+      <c t="n" s="1" r="T12"/>
+      <c t="n" s="1" r="U12"/>
+      <c t="s" s="15" r="V12">
         <v>39</v>
       </c>
-      <c t="n" r="W12" s="1"/>
-      <c t="s" r="X12" s="1">
+      <c t="n" s="1" r="W12"/>
+      <c t="s" s="1" r="X12">
         <v>40</v>
       </c>
-      <c t="s" r="Y12" s="1">
+      <c t="s" s="1" r="Y12">
         <v>41</v>
       </c>
-      <c t="n" r="Z12" s="1"/>
-      <c t="n" r="AA12" s="22"/>
+      <c t="n" s="1" r="Z12"/>
+      <c t="n" s="22" r="AA12"/>
       <c t="n" r="AB12">
         <v>8</v>
       </c>
-      <c t="s" r="AC12" s="16">
+      <c t="s" s="16" r="AC12">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use suggested values for lookup
- update sample and result files
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -13,7 +13,7 @@
     <s:definedName name="lookupexp_mea_tech_name">'lookup'!$A$19:$A$62</s:definedName>
     <s:definedName name="lookupexp_type_name">'lookup'!$A$1:$A$18</s:definedName>
     <s:definedName name="lookupsample_type_name">'lookup'!$A$75:$A$104</s:definedName>
-    <s:definedName name="lookupvirus_strain">'lookup'!$A$63:$A$74</s:definedName>
+    <s:definedName name="lookupvirus_strain">'lookup'!$B$1:$B$6</s:definedName>
   </s:definedNames>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="162">
   <si>
     <t>hai</t>
   </si>
@@ -416,10 +416,19 @@
     <t>Cellular_Activity</t>
   </si>
   <si>
+    <t>Influenza A virus (A/Victoria/361/2011(H3N2))</t>
+  </si>
+  <si>
     <t>Cellular_Phenotype</t>
   </si>
   <si>
+    <t>Influenza B virus (B/Brisbane/60/2008)</t>
+  </si>
+  <si>
     <t>Cellular_Quantification</t>
+  </si>
+  <si>
+    <t>Influenza B virus (B/Massachusetts/02/2012)</t>
   </si>
   <si>
     <t>Cytokine_Quantification</t>
@@ -921,7 +930,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -980,7 +989,6 @@
     <xf applyAlignment="1" borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1321,21 +1329,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
@@ -1349,571 +1357,571 @@
     <col customWidth="1" max="29" min="28" width="13.5"/>
   </cols>
   <sheetData>
-    <row spans="1:29" ht="38.25" customHeight="1" r="1">
-      <c t="s" s="2" r="A1">
+    <row customHeight="1" ht="38.25" r="1" spans="1:29">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:29" ht="51" customHeight="1" r="2">
-      <c t="s" s="1" r="A2">
+    <row customHeight="1" ht="51" r="2" spans="1:29">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:29" ht="63.75" customHeight="1" r="3">
-      <c t="s" s="4" r="A3">
+    <row customHeight="1" ht="63.75" r="3" spans="1:29">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="7" r="B3">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="9" r="C3">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="11" r="D3">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="7" r="E3">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="7" r="F3">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="6" r="G3">
+      <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="6" r="H3">
+      <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="6" r="I3">
+      <c r="I3" s="6" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="3" r="J3">
+      <c r="J3" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="K3">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="9" r="L3">
+      <c r="L3" s="9" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="9" r="M3">
+      <c r="M3" s="9" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="9" r="N3">
+      <c r="N3" s="9" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="8" r="O3">
+      <c r="O3" s="8" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="8" r="P3">
+      <c r="P3" s="8" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="8" r="Q3">
+      <c r="Q3" s="8" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="9" r="R3">
+      <c r="R3" s="9" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="9" r="S3">
+      <c r="S3" s="9" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="9" r="T3">
+      <c r="T3" s="9" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="8" r="U3">
+      <c r="U3" s="8" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="11" r="V3">
+      <c r="V3" s="11" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="10" r="W3">
+      <c r="W3" s="10" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="11" r="X3">
+      <c r="X3" s="11" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="11" r="Y3">
+      <c r="Y3" s="11" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="5" r="Z3">
+      <c r="Z3" s="5" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="2" r="AA3">
+      <c r="AA3" s="2" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="2" r="AB3">
+      <c r="AB3" s="2" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="3" r="AC3">
+      <c r="AC3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="4">
-      <c t="n" s="1" r="A4"/>
-      <c t="s" r="B4">
+    <row customHeight="1" ht="24" r="4" spans="1:29">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="14" r="D4">
+      <c r="D4" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E4">
+      <c r="E4" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F4">
+      <c r="F4" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G4"/>
-      <c t="n" s="1" r="H4"/>
-      <c t="n" s="1" r="I4"/>
-      <c t="n" s="1" r="J4"/>
-      <c t="s" s="14" r="K4">
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L4"/>
-      <c t="n" s="1" r="M4"/>
-      <c t="n" s="1" r="N4"/>
-      <c t="n" s="1" r="O4"/>
-      <c t="n" s="1" r="P4"/>
-      <c t="n" s="1" r="Q4"/>
-      <c t="n" s="1" r="R4"/>
-      <c t="n" s="1" r="S4"/>
-      <c t="n" s="1" r="T4"/>
-      <c t="n" s="1" r="U4"/>
-      <c t="s" s="15" r="V4">
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
+      <c r="T4" s="1" t="n"/>
+      <c r="U4" s="1" t="n"/>
+      <c r="V4" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W4"/>
-      <c t="s" s="1" r="X4">
+      <c r="W4" s="1" t="n"/>
+      <c r="X4" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y4">
+      <c r="Y4" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z4"/>
-      <c t="s" s="17" r="AA4">
+      <c r="Z4" s="1" t="n"/>
+      <c r="AA4" s="17" t="s">
         <v>42</v>
       </c>
-      <c t="n" r="AB4">
+      <c r="AB4" t="n">
         <v>16</v>
       </c>
-      <c t="s" s="16" r="AC4">
+      <c r="AC4" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="5">
-      <c t="n" s="1" r="A5"/>
-      <c t="s" r="B5">
+    <row customHeight="1" ht="24" r="5" spans="1:29">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="14" r="D5">
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E5">
+      <c r="E5" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F5">
+      <c r="F5" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G5"/>
-      <c t="n" s="1" r="H5"/>
-      <c t="n" s="1" r="I5"/>
-      <c t="n" s="1" r="J5"/>
-      <c t="s" s="14" r="K5">
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+      <c r="J5" s="1" t="n"/>
+      <c r="K5" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L5"/>
-      <c t="n" s="1" r="M5"/>
-      <c t="n" s="1" r="N5"/>
-      <c t="n" s="1" r="O5"/>
-      <c t="n" s="1" r="P5"/>
-      <c t="n" s="1" r="Q5"/>
-      <c t="n" s="1" r="R5"/>
-      <c t="n" s="1" r="S5"/>
-      <c t="n" s="1" r="T5"/>
-      <c t="n" s="1" r="U5"/>
-      <c t="s" s="15" r="V5">
+      <c r="L5" s="1" t="n"/>
+      <c r="M5" s="1" t="n"/>
+      <c r="N5" s="1" t="n"/>
+      <c r="O5" s="1" t="n"/>
+      <c r="P5" s="1" t="n"/>
+      <c r="Q5" s="1" t="n"/>
+      <c r="R5" s="1" t="n"/>
+      <c r="S5" s="1" t="n"/>
+      <c r="T5" s="1" t="n"/>
+      <c r="U5" s="1" t="n"/>
+      <c r="V5" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W5"/>
-      <c t="s" s="1" r="X5">
+      <c r="W5" s="1" t="n"/>
+      <c r="X5" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y5">
+      <c r="Y5" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z5"/>
-      <c t="s" s="18" r="AA5">
+      <c r="Z5" s="1" t="n"/>
+      <c r="AA5" s="18" t="s">
         <v>42</v>
       </c>
-      <c t="n" r="AB5">
+      <c r="AB5" t="n">
         <v>64</v>
       </c>
-      <c t="s" s="16" r="AC5">
+      <c r="AC5" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="6">
-      <c t="n" s="1" r="A6"/>
-      <c t="s" r="B6">
+    <row customHeight="1" ht="24" r="6" spans="1:29">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="14" r="D6">
+      <c r="D6" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E6">
+      <c r="E6" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F6">
+      <c r="F6" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G6"/>
-      <c t="n" s="1" r="H6"/>
-      <c t="n" s="1" r="I6"/>
-      <c t="n" s="1" r="J6"/>
-      <c t="s" s="14" r="K6">
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L6"/>
-      <c t="n" s="1" r="M6"/>
-      <c t="n" s="1" r="N6"/>
-      <c t="n" s="1" r="O6"/>
-      <c t="n" s="1" r="P6"/>
-      <c t="n" s="1" r="Q6"/>
-      <c t="n" s="1" r="R6"/>
-      <c t="n" s="1" r="S6"/>
-      <c t="n" s="1" r="T6"/>
-      <c t="n" s="1" r="U6"/>
-      <c t="s" s="15" r="V6">
+      <c r="L6" s="1" t="n"/>
+      <c r="M6" s="1" t="n"/>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+      <c r="P6" s="1" t="n"/>
+      <c r="Q6" s="1" t="n"/>
+      <c r="R6" s="1" t="n"/>
+      <c r="S6" s="1" t="n"/>
+      <c r="T6" s="1" t="n"/>
+      <c r="U6" s="1" t="n"/>
+      <c r="V6" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W6"/>
-      <c t="s" s="1" r="X6">
+      <c r="W6" s="1" t="n"/>
+      <c r="X6" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y6">
+      <c r="Y6" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z6"/>
-      <c t="s" s="19" r="AA6">
+      <c r="Z6" s="1" t="n"/>
+      <c r="AA6" s="19" t="s">
         <v>48</v>
       </c>
-      <c t="n" r="AB6">
+      <c r="AB6" t="n">
         <v>256</v>
       </c>
-      <c t="s" s="16" r="AC6">
+      <c r="AC6" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="7">
-      <c t="n" s="1" r="A7"/>
-      <c t="s" r="B7">
+    <row customHeight="1" ht="24" r="7" spans="1:29">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="14" r="D7">
+      <c r="D7" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E7">
+      <c r="E7" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F7">
+      <c r="F7" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G7"/>
-      <c t="n" s="1" r="H7"/>
-      <c t="n" s="1" r="I7"/>
-      <c t="n" s="1" r="J7"/>
-      <c t="s" s="14" r="K7">
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L7"/>
-      <c t="n" s="1" r="M7"/>
-      <c t="n" s="1" r="N7"/>
-      <c t="n" s="1" r="O7"/>
-      <c t="n" s="1" r="P7"/>
-      <c t="n" s="1" r="Q7"/>
-      <c t="n" s="1" r="R7"/>
-      <c t="n" s="1" r="S7"/>
-      <c t="n" s="1" r="T7"/>
-      <c t="n" s="1" r="U7"/>
-      <c t="s" s="15" r="V7">
+      <c r="L7" s="1" t="n"/>
+      <c r="M7" s="1" t="n"/>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="n"/>
+      <c r="P7" s="1" t="n"/>
+      <c r="Q7" s="1" t="n"/>
+      <c r="R7" s="1" t="n"/>
+      <c r="S7" s="1" t="n"/>
+      <c r="T7" s="1" t="n"/>
+      <c r="U7" s="1" t="n"/>
+      <c r="V7" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W7"/>
-      <c t="s" s="1" r="X7">
+      <c r="W7" s="1" t="n"/>
+      <c r="X7" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y7">
+      <c r="Y7" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z7"/>
-      <c t="s" s="19" r="AA7">
+      <c r="Z7" s="1" t="n"/>
+      <c r="AA7" s="19" t="s">
         <v>50</v>
       </c>
-      <c t="n" r="AB7">
+      <c r="AB7" t="n">
         <v>128</v>
       </c>
-      <c t="s" s="16" r="AC7">
+      <c r="AC7" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="8">
-      <c t="s" r="B8">
+    <row customHeight="1" ht="24" r="8" spans="1:29">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="14" r="D8">
+      <c r="D8" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E8">
+      <c r="E8" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F8">
+      <c r="F8" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G8"/>
-      <c t="s" s="14" r="K8">
+      <c r="G8" s="1" t="n"/>
+      <c r="K8" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="15" r="V8">
+      <c r="V8" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W8"/>
-      <c t="s" s="1" r="X8">
+      <c r="W8" s="1" t="n"/>
+      <c r="X8" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y8">
+      <c r="Y8" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="19" r="AA8">
+      <c r="AA8" s="19" t="s">
         <v>53</v>
       </c>
-      <c t="n" r="AB8">
+      <c r="AB8" t="n">
         <v>64</v>
       </c>
-      <c t="s" s="16" r="AC8">
+      <c r="AC8" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="9">
-      <c t="s" r="B9">
+    <row customHeight="1" ht="24" r="9" spans="1:29">
+      <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="14" r="D9">
+      <c r="D9" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E9">
+      <c r="E9" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F9">
+      <c r="F9" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G9"/>
-      <c t="s" s="14" r="K9">
+      <c r="G9" s="1" t="n"/>
+      <c r="K9" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="15" r="V9">
+      <c r="V9" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W9"/>
-      <c t="s" s="1" r="X9">
+      <c r="W9" s="1" t="n"/>
+      <c r="X9" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y9">
+      <c r="Y9" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="20" r="AA9">
+      <c r="AA9" s="19" t="s">
         <v>56</v>
       </c>
-      <c t="n" r="AB9">
+      <c r="AB9" t="n">
         <v>8</v>
       </c>
-      <c t="s" s="16" r="AC9">
+      <c r="AC9" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="10">
-      <c t="n" s="1" r="A10"/>
-      <c t="s" r="B10">
+    <row customHeight="1" ht="24" r="10" spans="1:29">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="14" r="D10">
+      <c r="D10" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E10">
+      <c r="E10" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F10">
+      <c r="F10" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G10"/>
-      <c t="n" s="1" r="H10"/>
-      <c t="n" s="1" r="I10"/>
-      <c t="n" s="1" r="J10"/>
-      <c t="s" s="14" r="K10">
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L10"/>
-      <c t="n" s="1" r="M10"/>
-      <c t="n" s="1" r="N10"/>
-      <c t="n" s="1" r="O10"/>
-      <c t="n" s="1" r="P10"/>
-      <c t="n" s="1" r="Q10"/>
-      <c t="n" s="1" r="R10"/>
-      <c t="n" s="1" r="S10"/>
-      <c t="n" s="1" r="T10"/>
-      <c t="n" s="1" r="U10"/>
-      <c t="s" s="15" r="V10">
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+      <c r="O10" s="1" t="n"/>
+      <c r="P10" s="1" t="n"/>
+      <c r="Q10" s="1" t="n"/>
+      <c r="R10" s="1" t="n"/>
+      <c r="S10" s="1" t="n"/>
+      <c r="T10" s="1" t="n"/>
+      <c r="U10" s="1" t="n"/>
+      <c r="V10" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W10"/>
-      <c t="s" s="1" r="X10">
+      <c r="W10" s="1" t="n"/>
+      <c r="X10" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y10">
+      <c r="Y10" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z10"/>
-      <c t="s" s="21" r="AA10">
+      <c r="Z10" s="1" t="n"/>
+      <c r="AA10" s="20" t="s">
         <v>60</v>
       </c>
-      <c t="n" r="AB10">
+      <c r="AB10" t="n">
         <v>32</v>
       </c>
-      <c t="s" s="16" r="AC10">
+      <c r="AC10" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="11">
-      <c t="n" s="1" r="A11"/>
-      <c t="s" r="B11">
+    <row customHeight="1" ht="24" r="11" spans="1:29">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" t="s">
         <v>61</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="14" r="D11">
+      <c r="D11" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E11">
+      <c r="E11" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F11">
+      <c r="F11" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G11"/>
-      <c t="n" s="1" r="H11"/>
-      <c t="n" s="1" r="I11"/>
-      <c t="n" s="1" r="J11"/>
-      <c t="s" s="14" r="K11">
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="1" t="n"/>
+      <c r="K11" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L11"/>
-      <c t="n" s="1" r="M11"/>
-      <c t="n" s="1" r="N11"/>
-      <c t="n" s="1" r="O11"/>
-      <c t="n" s="1" r="P11"/>
-      <c t="n" s="1" r="Q11"/>
-      <c t="n" s="1" r="R11"/>
-      <c t="n" s="1" r="S11"/>
-      <c t="n" s="1" r="T11"/>
-      <c t="n" s="1" r="U11"/>
-      <c t="s" s="15" r="V11">
+      <c r="L11" s="1" t="n"/>
+      <c r="M11" s="1" t="n"/>
+      <c r="N11" s="1" t="n"/>
+      <c r="O11" s="1" t="n"/>
+      <c r="P11" s="1" t="n"/>
+      <c r="Q11" s="1" t="n"/>
+      <c r="R11" s="1" t="n"/>
+      <c r="S11" s="1" t="n"/>
+      <c r="T11" s="1" t="n"/>
+      <c r="U11" s="1" t="n"/>
+      <c r="V11" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W11"/>
-      <c t="s" s="1" r="X11">
+      <c r="W11" s="1" t="n"/>
+      <c r="X11" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y11">
+      <c r="Y11" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z11"/>
-      <c t="s" s="22" r="AA11">
+      <c r="Z11" s="1" t="n"/>
+      <c r="AA11" s="21" t="s">
         <v>63</v>
       </c>
-      <c t="n" r="AB11">
+      <c r="AB11" t="n">
         <v>8</v>
       </c>
-      <c t="s" s="16" r="AC11">
+      <c r="AC11" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:29" ht="24" customHeight="1" r="12">
-      <c t="n" s="1" r="A12"/>
-      <c t="s" r="B12">
+    <row customHeight="1" ht="24" r="12" spans="1:29">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="14" r="D12">
+      <c r="D12" s="14" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="E12">
+      <c r="E12" s="12" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="13" r="F12">
+      <c r="F12" s="13" t="s">
         <v>37</v>
       </c>
-      <c t="n" s="1" r="G12"/>
-      <c t="n" s="1" r="H12"/>
-      <c t="n" s="1" r="I12"/>
-      <c t="n" s="1" r="J12"/>
-      <c t="s" s="14" r="K12">
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="1" t="n"/>
+      <c r="K12" s="14" t="s">
         <v>38</v>
       </c>
-      <c t="n" s="1" r="L12"/>
-      <c t="n" s="1" r="M12"/>
-      <c t="n" s="1" r="N12"/>
-      <c t="n" s="1" r="O12"/>
-      <c t="n" s="1" r="P12"/>
-      <c t="n" s="1" r="Q12"/>
-      <c t="n" s="1" r="R12"/>
-      <c t="n" s="1" r="S12"/>
-      <c t="n" s="1" r="T12"/>
-      <c t="n" s="1" r="U12"/>
-      <c t="s" s="15" r="V12">
+      <c r="L12" s="1" t="n"/>
+      <c r="M12" s="1" t="n"/>
+      <c r="N12" s="1" t="n"/>
+      <c r="O12" s="1" t="n"/>
+      <c r="P12" s="1" t="n"/>
+      <c r="Q12" s="1" t="n"/>
+      <c r="R12" s="1" t="n"/>
+      <c r="S12" s="1" t="n"/>
+      <c r="T12" s="1" t="n"/>
+      <c r="U12" s="1" t="n"/>
+      <c r="V12" s="15" t="s">
         <v>39</v>
       </c>
-      <c t="n" s="1" r="W12"/>
-      <c t="s" s="1" r="X12">
+      <c r="W12" s="1" t="n"/>
+      <c r="X12" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="Y12">
+      <c r="Y12" s="1" t="s">
         <v>41</v>
       </c>
-      <c t="n" s="1" r="Z12"/>
-      <c t="n" s="22" r="AA12"/>
-      <c t="n" r="AB12">
+      <c r="Z12" s="1" t="n"/>
+      <c r="AA12" s="21" t="n"/>
+      <c r="AB12" t="n">
         <v>8</v>
       </c>
-      <c t="s" s="16" r="AC12">
+      <c r="AC12" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1934,14 +1942,14 @@
     <dataValidation allowBlank="1" error="Required value was not selected" errorTitle="Measurement Technique" prompt="Please choose required value from the list" promptTitle="Measurement Technique" showErrorMessage="1" showInputMessage="1" sqref="Y4:Y12" type="list">
       <formula1>lookupexp_mea_tech_name</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Preferred value was not selected" errorStyle="information" errorTitle="Virus Strain" prompt="Please choose preferred value from the list" promptTitle="Virus Strain" showErrorMessage="1" showInputMessage="1" sqref="AA4:AA8 AA10:AA12" type="list">
+    <dataValidation allowBlank="1" error="Preferred value was not selected" errorStyle="information" errorTitle="Virus Strain" prompt="Please choose preferred value from the list" promptTitle="Virus Strain" showErrorMessage="1" showInputMessage="1" sqref="AA4:AA12" type="list">
       <formula1>lookupvirus_strain</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Please choose a value from the list." errorStyle="information" errorTitle="Choose from the list" prompt="Please choose a value from the list." promptTitle="Choose an array from the list" showErrorMessage="1" showInputMessage="1" sqref="E4:E12"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="commentsvml"/>
 </worksheet>
 </file>
 
@@ -1951,7 +1959,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A104"/>
+  <dimension ref="A2:B104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1959,504 +1967,516 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:1" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row spans="1:1" r="3">
-      <c t="s" r="A3">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row spans="1:1" r="4">
-      <c t="s" r="A4">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row spans="1:1" r="5">
-      <c t="s" r="A5">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row spans="1:1" r="6">
-      <c t="s" r="A6">
+      <c r="B4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row spans="1:1" r="7">
-      <c t="s" r="A7">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row spans="1:1" r="8">
-      <c t="s" r="A8">
+      <c r="B5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row spans="1:1" r="9">
-      <c t="s" r="A9">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row spans="1:1" r="10">
-      <c t="s" r="A10">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row spans="1:1" r="11">
-      <c t="s" r="A11">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row spans="1:1" r="12">
-      <c t="s" r="A12">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row spans="1:1" r="13">
-      <c t="s" r="A13">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row spans="1:1" r="14">
-      <c t="s" r="A14">
-        <v>75</v>
-      </c>
-    </row>
-    <row spans="1:1" r="15">
-      <c t="s" r="A15">
-        <v>76</v>
-      </c>
-    </row>
-    <row spans="1:1" r="16">
-      <c t="s" r="A16">
-        <v>77</v>
-      </c>
-    </row>
-    <row spans="1:1" r="17">
-      <c t="s" r="A17">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row spans="1:1" r="18">
-      <c t="s" r="A18">
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row spans="1:1" r="20">
-      <c t="s" r="A20">
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row spans="1:1" r="21">
-      <c t="s" r="A21">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row spans="1:1" r="22">
-      <c t="s" r="A22">
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row spans="1:1" r="23">
-      <c t="s" r="A23">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row spans="1:1" r="24">
-      <c t="s" r="A24">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row spans="1:1" r="25">
-      <c t="s" r="A25">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row spans="1:1" r="26">
-      <c t="s" r="A26">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row spans="1:1" r="27">
-      <c t="s" r="A27">
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row spans="1:1" r="28">
-      <c t="s" r="A28">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row spans="1:1" r="29">
-      <c t="s" r="A29">
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row spans="1:1" r="30">
-      <c t="s" r="A30">
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row spans="1:1" r="31">
-      <c t="s" r="A31">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row spans="1:1" r="32">
-      <c t="s" r="A32">
-        <v>91</v>
-      </c>
-    </row>
-    <row spans="1:1" r="33">
-      <c t="s" r="A33">
-        <v>92</v>
-      </c>
-    </row>
-    <row spans="1:1" r="34">
-      <c t="s" r="A34">
-        <v>93</v>
-      </c>
-    </row>
-    <row spans="1:1" r="35">
-      <c t="s" r="A35">
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row spans="1:1" r="36">
-      <c t="s" r="A36">
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row spans="1:1" r="37">
-      <c t="s" r="A37">
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row spans="1:1" r="38">
-      <c t="s" r="A38">
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row spans="1:1" r="39">
-      <c t="s" r="A39">
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row spans="1:1" r="40">
-      <c t="s" r="A40">
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row spans="1:1" r="41">
-      <c t="s" r="A41">
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row spans="1:1" r="42">
-      <c t="s" r="A42">
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row spans="1:1" r="43">
-      <c t="s" r="A43">
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>102</v>
       </c>
     </row>
-    <row spans="1:1" r="44">
-      <c t="s" r="A44">
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>103</v>
       </c>
     </row>
-    <row spans="1:1" r="45">
-      <c t="s" r="A45">
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row spans="1:1" r="46">
-      <c t="s" r="A46">
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row spans="1:1" r="47">
-      <c t="s" r="A47">
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row spans="1:1" r="48">
-      <c t="s" r="A48">
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row spans="1:1" r="49">
-      <c t="s" r="A49">
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row spans="1:1" r="50">
-      <c t="s" r="A50">
-        <v>75</v>
-      </c>
-    </row>
-    <row spans="1:1" r="51">
-      <c t="s" r="A51">
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>109</v>
       </c>
     </row>
-    <row spans="1:1" r="52">
-      <c t="s" r="A52">
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>110</v>
       </c>
     </row>
-    <row spans="1:1" r="53">
-      <c t="s" r="A53">
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>111</v>
       </c>
     </row>
-    <row spans="1:1" r="54">
-      <c t="s" r="A54">
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>112</v>
       </c>
     </row>
-    <row spans="1:1" r="55">
-      <c t="s" r="A55">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>113</v>
       </c>
     </row>
-    <row spans="1:1" r="56">
-      <c t="s" r="A56">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>114</v>
       </c>
     </row>
-    <row spans="1:1" r="57">
-      <c t="s" r="A57">
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>115</v>
       </c>
     </row>
-    <row spans="1:1" r="58">
-      <c t="s" r="A58">
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>116</v>
       </c>
     </row>
-    <row spans="1:1" r="59">
-      <c t="s" r="A59">
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>117</v>
       </c>
     </row>
-    <row spans="1:1" r="60">
-      <c t="s" r="A60">
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>118</v>
       </c>
     </row>
-    <row spans="1:1" r="61">
-      <c t="s" r="A61">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>119</v>
       </c>
     </row>
-    <row spans="1:1" r="62">
-      <c t="s" r="A62">
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>120</v>
       </c>
     </row>
-    <row spans="1:1" r="64">
-      <c t="s" r="A64">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>121</v>
       </c>
     </row>
-    <row spans="1:1" r="65">
-      <c t="s" r="A65">
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
         <v>122</v>
       </c>
     </row>
-    <row spans="1:1" r="66">
-      <c t="s" r="A66">
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>123</v>
       </c>
     </row>
-    <row spans="1:1" r="67">
-      <c t="s" r="A67">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>124</v>
       </c>
     </row>
-    <row spans="1:1" r="68">
-      <c t="s" r="A68">
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row spans="1:1" r="69">
-      <c t="s" r="A69">
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
         <v>126</v>
       </c>
     </row>
-    <row spans="1:1" r="70">
-      <c t="s" r="A70">
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
         <v>127</v>
       </c>
     </row>
-    <row spans="1:1" r="71">
-      <c t="s" r="A71">
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
         <v>56</v>
       </c>
     </row>
-    <row spans="1:1" r="72">
-      <c t="s" r="A72">
-        <v>128</v>
-      </c>
-    </row>
-    <row spans="1:1" r="73">
-      <c t="s" r="A73">
-        <v>129</v>
-      </c>
-    </row>
-    <row spans="1:1" r="74">
-      <c t="s" r="A74">
-        <v>130</v>
-      </c>
-    </row>
-    <row spans="1:1" r="76">
-      <c t="s" r="A76">
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>131</v>
       </c>
     </row>
-    <row spans="1:1" r="77">
-      <c t="s" r="A77">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>132</v>
       </c>
     </row>
-    <row spans="1:1" r="78">
-      <c t="s" r="A78">
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>133</v>
       </c>
     </row>
-    <row spans="1:1" r="79">
-      <c t="s" r="A79">
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
         <v>134</v>
       </c>
     </row>
-    <row spans="1:1" r="80">
-      <c t="s" r="A80">
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
         <v>135</v>
       </c>
     </row>
-    <row spans="1:1" r="81">
-      <c t="s" r="A81">
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
         <v>136</v>
       </c>
     </row>
-    <row spans="1:1" r="82">
-      <c t="s" r="A82">
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
         <v>137</v>
       </c>
     </row>
-    <row spans="1:1" r="83">
-      <c t="s" r="A83">
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
         <v>138</v>
       </c>
     </row>
-    <row spans="1:1" r="84">
-      <c t="s" r="A84">
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>139</v>
       </c>
     </row>
-    <row spans="1:1" r="85">
-      <c t="s" r="A85">
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
         <v>140</v>
       </c>
     </row>
-    <row spans="1:1" r="86">
-      <c t="s" r="A86">
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
         <v>141</v>
       </c>
     </row>
-    <row spans="1:1" r="87">
-      <c t="s" r="A87">
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
         <v>142</v>
       </c>
     </row>
-    <row spans="1:1" r="88">
-      <c t="s" r="A88">
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
         <v>143</v>
       </c>
     </row>
-    <row spans="1:1" r="89">
-      <c t="s" r="A89">
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
         <v>144</v>
       </c>
     </row>
-    <row spans="1:1" r="90">
-      <c t="s" r="A90">
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
         <v>145</v>
       </c>
     </row>
-    <row spans="1:1" r="91">
-      <c t="s" r="A91">
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
         <v>146</v>
       </c>
     </row>
-    <row spans="1:1" r="92">
-      <c t="s" r="A92">
-        <v>75</v>
-      </c>
-    </row>
-    <row spans="1:1" r="93">
-      <c t="s" r="A93">
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
         <v>147</v>
       </c>
     </row>
-    <row spans="1:1" r="94">
-      <c t="s" r="A94">
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
         <v>148</v>
       </c>
     </row>
-    <row spans="1:1" r="95">
-      <c t="s" r="A95">
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
         <v>149</v>
       </c>
     </row>
-    <row spans="1:1" r="96">
-      <c t="s" r="A96">
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
         <v>150</v>
       </c>
     </row>
-    <row spans="1:1" r="97">
-      <c t="s" r="A97">
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row spans="1:1" r="98">
-      <c t="s" r="A98">
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
         <v>152</v>
       </c>
     </row>
-    <row spans="1:1" r="99">
-      <c t="s" r="A99">
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
         <v>153</v>
       </c>
     </row>
-    <row spans="1:1" r="100">
-      <c t="s" r="A100">
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>154</v>
       </c>
     </row>
-    <row spans="1:1" r="101">
-      <c t="s" r="A101">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row spans="1:1" r="102">
-      <c t="s" r="A102">
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
         <v>156</v>
       </c>
     </row>
-    <row spans="1:1" r="103">
-      <c t="s" r="A103">
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
         <v>157</v>
       </c>
     </row>
-    <row spans="1:1" r="104">
-      <c t="s" r="A104">
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>